<commit_message>
Add comprehensive weighting method analysis plots
- Added 5 suites of weighting comparison plots:
  1. RMSE by weighting method across validity schemes (All, ANESRake-Full, ANESRake-Restricted)
  2. RMSE by weighting method by variable class (Demographic, Voting, Candidate Choice)
  3. RMSE reduction by office comparing unweighted vs CES-weighted estimates
  4. RMSE progression by year (with variant excluding voter data)
  5. ANESRake-Full vs ANESRake-Restricted validity scheme comparison

- All plots use grouped bar charts with years on x-axis for temporal trends
- Added 5 new cells to figuresHQ.ipynb with placeholder documentation
- Generated output files ready for inclusion in analysis
</commit_message>
<xml_diff>
--- a/tables_and_figures/output/anesrake_full_vs_restricted_comparison.xlsx
+++ b/tables_and_figures/output/anesrake_full_vs_restricted_comparison.xlsx
@@ -481,10 +481,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>18.59763052456585</v>
+        <v>18.54691586254667</v>
       </c>
       <c r="C4" t="n">
-        <v>11.93973333493228</v>
+        <v>11.97649572186662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>